<commit_message>
Update on 20250621 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/IPV6直播源汇总/黑龙江移动-域名版.xlsx
+++ b/直播源汇总文档/IPV6直播源汇总/黑龙江移动-域名版.xlsx
@@ -1129,12 +1129,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>鸡西公共</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>鸡西新闻综合</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸡西安全生活</t>
   </si>
 </sst>
 </file>
@@ -3821,7 +3820,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" t="s">
         <v>208</v>
@@ -3835,7 +3834,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B45" t="s">
         <v>208</v>

</xml_diff>